<commit_message>
Adding OLS for External and Internal Losses as well
</commit_message>
<xml_diff>
--- a/ndiff_results.xlsx
+++ b/ndiff_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gourav/workspace/qafm/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CE3EA27-078A-504D-86B5-409E54A8A531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D1070138-BCC2-CE4B-85EB-076F93CA0065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2943" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2943" uniqueCount="593">
   <si>
     <t>DATE</t>
   </si>
@@ -1795,9 +1795,6 @@
   </si>
   <si>
     <t>Grand Total</t>
-  </si>
-  <si>
-    <t>Column Labels</t>
   </si>
   <si>
     <t>Sum of ndiffs</t>
@@ -5896,7 +5893,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Attributes">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Attributes" colHeaderCaption="Transformation">
   <location ref="A3:Z30" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -5930,6 +5927,7 @@
     </pivotField>
     <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
       <items count="10">
+        <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item m="1" x="6"/>
@@ -5939,17 +5937,16 @@
         <item x="3"/>
         <item x="4"/>
         <item m="1" x="5"/>
-        <item x="0"/>
       </items>
     </pivotField>
     <pivotField axis="axisCol" showAll="0">
       <items count="7">
+        <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
         <item m="1" x="5"/>
-        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -6054,7 +6051,7 @@
       <x v="3"/>
     </i>
     <i r="1">
-      <x v="5"/>
+      <x v="4"/>
     </i>
     <i>
       <x v="1"/>
@@ -6070,10 +6067,10 @@
       <x v="3"/>
     </i>
     <i r="1">
-      <x v="5"/>
+      <x v="4"/>
     </i>
     <i>
-      <x v="6"/>
+      <x v="2"/>
       <x/>
     </i>
     <i r="1">
@@ -6086,7 +6083,7 @@
       <x v="3"/>
     </i>
     <i r="1">
-      <x v="5"/>
+      <x v="4"/>
     </i>
     <i>
       <x v="7"/>
@@ -6102,10 +6099,10 @@
       <x v="3"/>
     </i>
     <i r="1">
-      <x v="5"/>
+      <x v="4"/>
     </i>
     <i>
-      <x v="9"/>
+      <x v="8"/>
       <x/>
     </i>
     <i r="1">
@@ -6118,7 +6115,7 @@
       <x v="3"/>
     </i>
     <i r="1">
-      <x v="5"/>
+      <x v="4"/>
     </i>
   </colItems>
   <dataFields count="1">
@@ -6436,7 +6433,7 @@
   <dimension ref="A1:VD2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:VD2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9911,22 +9908,22 @@
   <dimension ref="A3:Z30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="Z29" sqref="A3:Z29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="11" width="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="16" width="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5" bestFit="1" customWidth="1"/>
     <col min="18" max="21" width="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="26" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="26" width="3" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="7" bestFit="1" customWidth="1"/>
     <col min="29" max="31" width="3" bestFit="1" customWidth="1"/>
@@ -9938,107 +9935,107 @@
   <sheetData>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>591</v>
+      </c>
+      <c r="G4" t="s">
         <v>578</v>
       </c>
-      <c r="G4" t="s">
+      <c r="L4" t="s">
         <v>579</v>
       </c>
-      <c r="L4" t="s">
+      <c r="Q4" t="s">
         <v>580</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="V4" t="s">
         <v>581</v>
-      </c>
-      <c r="V4" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B5" t="s">
+        <v>590</v>
+      </c>
+      <c r="C5" t="s">
         <v>582</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>583</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>584</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>585</v>
       </c>
-      <c r="F5" t="s">
-        <v>591</v>
-      </c>
       <c r="G5" t="s">
+        <v>590</v>
+      </c>
+      <c r="H5" t="s">
         <v>582</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>583</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>584</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>585</v>
       </c>
-      <c r="K5" t="s">
-        <v>591</v>
-      </c>
       <c r="L5" t="s">
+        <v>590</v>
+      </c>
+      <c r="M5" t="s">
         <v>582</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>583</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>584</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>585</v>
       </c>
-      <c r="P5" t="s">
-        <v>591</v>
-      </c>
       <c r="Q5" t="s">
+        <v>590</v>
+      </c>
+      <c r="R5" t="s">
         <v>582</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>583</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>584</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>585</v>
       </c>
-      <c r="U5" t="s">
-        <v>591</v>
-      </c>
       <c r="V5" t="s">
+        <v>590</v>
+      </c>
+      <c r="W5" t="s">
         <v>582</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>583</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>584</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>585</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
@@ -10046,19 +10043,19 @@
         <v>14</v>
       </c>
       <c r="B6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -10106,19 +10103,19 @@
         <v>0</v>
       </c>
       <c r="V6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
@@ -10126,19 +10123,19 @@
         <v>10</v>
       </c>
       <c r="B7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -10171,22 +10168,22 @@
         <v>0</v>
       </c>
       <c r="Q7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U7" s="3">
         <v>0</v>
       </c>
       <c r="V7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W7" s="3">
         <v>1</v>
@@ -10205,7 +10202,9 @@
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -10229,28 +10228,26 @@
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
-      <c r="Z8" s="3">
-        <v>1</v>
-      </c>
+      <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -10298,19 +10295,19 @@
         <v>0</v>
       </c>
       <c r="V9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
@@ -10318,19 +10315,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="3">
         <v>0</v>
@@ -10375,22 +10372,22 @@
         <v>0</v>
       </c>
       <c r="U10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V10" s="3">
         <v>1</v>
       </c>
       <c r="W10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
@@ -10398,19 +10395,19 @@
         <v>9</v>
       </c>
       <c r="B11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
       </c>
       <c r="F11" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" s="3">
         <v>0</v>
@@ -10425,10 +10422,10 @@
         <v>0</v>
       </c>
       <c r="K11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" s="3">
         <v>0</v>
@@ -10437,10 +10434,10 @@
         <v>0</v>
       </c>
       <c r="O11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="3">
         <v>1</v>
@@ -10449,10 +10446,10 @@
         <v>1</v>
       </c>
       <c r="S11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U11" s="3">
         <v>1</v>
@@ -10467,7 +10464,7 @@
         <v>1</v>
       </c>
       <c r="Y11" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z11" s="3">
         <v>1</v>
@@ -10478,19 +10475,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="3">
         <v>0</v>
@@ -10538,19 +10535,19 @@
         <v>0</v>
       </c>
       <c r="V12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
@@ -10558,19 +10555,19 @@
         <v>7</v>
       </c>
       <c r="B13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="3">
         <v>0</v>
@@ -10618,19 +10615,19 @@
         <v>0</v>
       </c>
       <c r="V13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
@@ -10638,19 +10635,19 @@
         <v>11</v>
       </c>
       <c r="B14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="3">
         <v>0</v>
@@ -10698,19 +10695,19 @@
         <v>0</v>
       </c>
       <c r="V14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
@@ -10718,19 +10715,19 @@
         <v>20</v>
       </c>
       <c r="B15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="3">
         <v>0</v>
@@ -10778,19 +10775,19 @@
         <v>0</v>
       </c>
       <c r="V15" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W15" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X15" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y15" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z15" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
@@ -10798,19 +10795,19 @@
         <v>21</v>
       </c>
       <c r="B16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="3">
         <v>0</v>
@@ -10858,19 +10855,19 @@
         <v>0</v>
       </c>
       <c r="V16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
@@ -10878,19 +10875,19 @@
         <v>22</v>
       </c>
       <c r="B17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="3">
         <v>0</v>
@@ -10938,19 +10935,19 @@
         <v>0</v>
       </c>
       <c r="V17" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X17" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y17" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z17" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
@@ -11038,19 +11035,19 @@
         <v>8</v>
       </c>
       <c r="B19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="3">
         <v>0</v>
@@ -11098,19 +11095,19 @@
         <v>0</v>
       </c>
       <c r="V19" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W19" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X19" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y19" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z19" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
@@ -11118,19 +11115,19 @@
         <v>13</v>
       </c>
       <c r="B20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="3">
         <v>0</v>
@@ -11178,19 +11175,19 @@
         <v>0</v>
       </c>
       <c r="V20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
@@ -11198,19 +11195,19 @@
         <v>2</v>
       </c>
       <c r="B21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="3">
         <v>0</v>
@@ -11258,19 +11255,19 @@
         <v>0</v>
       </c>
       <c r="V21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
@@ -11278,19 +11275,19 @@
         <v>15</v>
       </c>
       <c r="B22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="3">
         <v>0</v>
@@ -11314,7 +11311,7 @@
         <v>0</v>
       </c>
       <c r="N22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O22" s="3">
         <v>0</v>
@@ -11332,25 +11329,25 @@
         <v>0</v>
       </c>
       <c r="T22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U22" s="3">
         <v>0</v>
       </c>
       <c r="V22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
@@ -11358,19 +11355,19 @@
         <v>18</v>
       </c>
       <c r="B23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="3">
         <v>0</v>
@@ -11388,16 +11385,16 @@
         <v>0</v>
       </c>
       <c r="L23" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N23" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O23" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P23" s="3">
         <v>0</v>
@@ -11406,31 +11403,31 @@
         <v>0</v>
       </c>
       <c r="R23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V23" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W23" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X23" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y23" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z23" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
@@ -11438,19 +11435,19 @@
         <v>3</v>
       </c>
       <c r="B24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="3">
         <v>0</v>
@@ -11498,19 +11495,19 @@
         <v>0</v>
       </c>
       <c r="V24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
@@ -11518,19 +11515,19 @@
         <v>19</v>
       </c>
       <c r="B25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="3">
         <v>0</v>
@@ -11548,49 +11545,49 @@
         <v>0</v>
       </c>
       <c r="L25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
@@ -11678,19 +11675,19 @@
         <v>5</v>
       </c>
       <c r="B27" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="3">
         <v>0</v>
@@ -11738,19 +11735,19 @@
         <v>0</v>
       </c>
       <c r="V27" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W27" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X27" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y27" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z27" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
@@ -11758,19 +11755,19 @@
         <v>16</v>
       </c>
       <c r="B28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="3">
         <v>0</v>
@@ -11815,22 +11812,22 @@
         <v>0</v>
       </c>
       <c r="U28" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V28" s="3">
         <v>1</v>
       </c>
       <c r="W28" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X28" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y28" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z28" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
@@ -11838,19 +11835,19 @@
         <v>12</v>
       </c>
       <c r="B29" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="3">
         <v>0</v>
@@ -11892,22 +11889,22 @@
         <v>0</v>
       </c>
       <c r="T29" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U29" s="3">
         <v>0</v>
       </c>
       <c r="V29" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W29" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X29" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y29" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z29" s="3">
         <v>1</v>
@@ -11918,19 +11915,19 @@
         <v>588</v>
       </c>
       <c r="B30" s="3">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C30" s="3">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D30" s="3">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E30" s="3">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="F30" s="3">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G30" s="3">
         <v>0</v>
@@ -11945,28 +11942,28 @@
         <v>0</v>
       </c>
       <c r="K30" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M30" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N30" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O30" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P30" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q30" s="3">
         <v>2</v>
       </c>
       <c r="R30" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S30" s="3">
         <v>2</v>
@@ -11978,19 +11975,19 @@
         <v>3</v>
       </c>
       <c r="V30" s="3">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="W30" s="3">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="X30" s="3">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="Y30" s="3">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="Z30" s="3">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -12038,10 +12035,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -12055,10 +12052,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -12072,10 +12069,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -12089,10 +12086,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -12106,10 +12103,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D6" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -12123,10 +12120,10 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D7" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -12140,10 +12137,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D8" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -12157,10 +12154,10 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D9" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -12174,10 +12171,10 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D10" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -12191,10 +12188,10 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D11" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -12208,10 +12205,10 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D12" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -12225,10 +12222,10 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D13" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -12242,10 +12239,10 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D14" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -12259,10 +12256,10 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D15" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -12276,10 +12273,10 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D16" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -12293,10 +12290,10 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D17" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -12310,10 +12307,10 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D18" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -12327,10 +12324,10 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D19" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -12344,10 +12341,10 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D20" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -12361,10 +12358,10 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D21" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -12378,10 +12375,10 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D22" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -12395,10 +12392,10 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D23" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -12412,10 +12409,10 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D24" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -12429,10 +12426,10 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D25" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -12449,7 +12446,7 @@
         <v>578</v>
       </c>
       <c r="D26" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -12466,7 +12463,7 @@
         <v>579</v>
       </c>
       <c r="D27" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -12483,7 +12480,7 @@
         <v>580</v>
       </c>
       <c r="D28" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -12500,7 +12497,7 @@
         <v>581</v>
       </c>
       <c r="D29" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -12517,7 +12514,7 @@
         <v>578</v>
       </c>
       <c r="D30" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -12534,7 +12531,7 @@
         <v>579</v>
       </c>
       <c r="D31" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -12551,7 +12548,7 @@
         <v>580</v>
       </c>
       <c r="D32" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -12568,7 +12565,7 @@
         <v>581</v>
       </c>
       <c r="D33" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -12585,7 +12582,7 @@
         <v>578</v>
       </c>
       <c r="D34" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -12602,7 +12599,7 @@
         <v>579</v>
       </c>
       <c r="D35" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -12619,7 +12616,7 @@
         <v>580</v>
       </c>
       <c r="D36" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -12636,7 +12633,7 @@
         <v>581</v>
       </c>
       <c r="D37" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -12653,7 +12650,7 @@
         <v>578</v>
       </c>
       <c r="D38" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -12670,7 +12667,7 @@
         <v>579</v>
       </c>
       <c r="D39" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -12687,7 +12684,7 @@
         <v>580</v>
       </c>
       <c r="D40" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -12704,7 +12701,7 @@
         <v>581</v>
       </c>
       <c r="D41" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -12721,7 +12718,7 @@
         <v>578</v>
       </c>
       <c r="D42" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -12738,7 +12735,7 @@
         <v>579</v>
       </c>
       <c r="D43" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -12755,7 +12752,7 @@
         <v>580</v>
       </c>
       <c r="D44" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -12772,7 +12769,7 @@
         <v>581</v>
       </c>
       <c r="D45" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -12789,7 +12786,7 @@
         <v>578</v>
       </c>
       <c r="D46" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -12806,7 +12803,7 @@
         <v>579</v>
       </c>
       <c r="D47" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -12823,7 +12820,7 @@
         <v>580</v>
       </c>
       <c r="D48" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -12840,7 +12837,7 @@
         <v>581</v>
       </c>
       <c r="D49" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -12857,7 +12854,7 @@
         <v>578</v>
       </c>
       <c r="D50" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -12874,7 +12871,7 @@
         <v>579</v>
       </c>
       <c r="D51" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -12891,7 +12888,7 @@
         <v>580</v>
       </c>
       <c r="D52" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -12908,7 +12905,7 @@
         <v>581</v>
       </c>
       <c r="D53" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -12925,7 +12922,7 @@
         <v>578</v>
       </c>
       <c r="D54" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -12942,7 +12939,7 @@
         <v>579</v>
       </c>
       <c r="D55" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -12959,7 +12956,7 @@
         <v>580</v>
       </c>
       <c r="D56" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -12976,7 +12973,7 @@
         <v>581</v>
       </c>
       <c r="D57" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -12993,7 +12990,7 @@
         <v>578</v>
       </c>
       <c r="D58" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -13010,7 +13007,7 @@
         <v>579</v>
       </c>
       <c r="D59" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -13027,7 +13024,7 @@
         <v>580</v>
       </c>
       <c r="D60" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -13044,7 +13041,7 @@
         <v>581</v>
       </c>
       <c r="D61" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -13061,7 +13058,7 @@
         <v>578</v>
       </c>
       <c r="D62" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -13078,7 +13075,7 @@
         <v>579</v>
       </c>
       <c r="D63" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -13095,7 +13092,7 @@
         <v>580</v>
       </c>
       <c r="D64" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -13112,7 +13109,7 @@
         <v>581</v>
       </c>
       <c r="D65" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -13129,7 +13126,7 @@
         <v>578</v>
       </c>
       <c r="D66" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E66">
         <v>0</v>
@@ -13146,7 +13143,7 @@
         <v>579</v>
       </c>
       <c r="D67" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E67">
         <v>0</v>
@@ -13163,7 +13160,7 @@
         <v>580</v>
       </c>
       <c r="D68" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -13180,7 +13177,7 @@
         <v>581</v>
       </c>
       <c r="D69" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -13197,7 +13194,7 @@
         <v>578</v>
       </c>
       <c r="D70" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -13214,7 +13211,7 @@
         <v>579</v>
       </c>
       <c r="D71" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -13231,7 +13228,7 @@
         <v>580</v>
       </c>
       <c r="D72" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E72">
         <v>0</v>
@@ -13248,7 +13245,7 @@
         <v>581</v>
       </c>
       <c r="D73" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E73">
         <v>0</v>
@@ -13265,7 +13262,7 @@
         <v>578</v>
       </c>
       <c r="D74" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -13282,7 +13279,7 @@
         <v>579</v>
       </c>
       <c r="D75" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -13299,7 +13296,7 @@
         <v>580</v>
       </c>
       <c r="D76" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -13316,7 +13313,7 @@
         <v>581</v>
       </c>
       <c r="D77" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E77">
         <v>0</v>
@@ -13333,7 +13330,7 @@
         <v>578</v>
       </c>
       <c r="D78" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E78">
         <v>0</v>
@@ -13350,7 +13347,7 @@
         <v>579</v>
       </c>
       <c r="D79" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -13367,7 +13364,7 @@
         <v>580</v>
       </c>
       <c r="D80" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -13384,7 +13381,7 @@
         <v>581</v>
       </c>
       <c r="D81" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -13401,7 +13398,7 @@
         <v>578</v>
       </c>
       <c r="D82" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -13418,7 +13415,7 @@
         <v>579</v>
       </c>
       <c r="D83" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -13435,7 +13432,7 @@
         <v>580</v>
       </c>
       <c r="D84" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -13452,7 +13449,7 @@
         <v>581</v>
       </c>
       <c r="D85" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E85">
         <v>0</v>
@@ -13469,7 +13466,7 @@
         <v>578</v>
       </c>
       <c r="D86" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E86">
         <v>0</v>
@@ -13486,7 +13483,7 @@
         <v>579</v>
       </c>
       <c r="D87" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E87">
         <v>0</v>
@@ -13503,7 +13500,7 @@
         <v>580</v>
       </c>
       <c r="D88" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E88">
         <v>0</v>
@@ -13520,7 +13517,7 @@
         <v>581</v>
       </c>
       <c r="D89" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E89">
         <v>1</v>
@@ -13537,7 +13534,7 @@
         <v>578</v>
       </c>
       <c r="D90" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E90">
         <v>0</v>
@@ -13554,7 +13551,7 @@
         <v>579</v>
       </c>
       <c r="D91" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E91">
         <v>0</v>
@@ -13571,7 +13568,7 @@
         <v>580</v>
       </c>
       <c r="D92" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E92">
         <v>0</v>
@@ -13588,7 +13585,7 @@
         <v>581</v>
       </c>
       <c r="D93" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E93">
         <v>0</v>
@@ -13605,7 +13602,7 @@
         <v>578</v>
       </c>
       <c r="D94" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E94">
         <v>0</v>
@@ -13622,7 +13619,7 @@
         <v>579</v>
       </c>
       <c r="D95" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E95">
         <v>0</v>
@@ -13639,7 +13636,7 @@
         <v>580</v>
       </c>
       <c r="D96" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E96">
         <v>0</v>
@@ -13656,7 +13653,7 @@
         <v>581</v>
       </c>
       <c r="D97" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E97">
         <v>0</v>
@@ -13673,7 +13670,7 @@
         <v>578</v>
       </c>
       <c r="D98" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E98">
         <v>0</v>
@@ -13690,7 +13687,7 @@
         <v>579</v>
       </c>
       <c r="D99" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E99">
         <v>0</v>
@@ -13707,7 +13704,7 @@
         <v>580</v>
       </c>
       <c r="D100" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -13724,7 +13721,7 @@
         <v>581</v>
       </c>
       <c r="D101" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E101">
         <v>0</v>
@@ -13741,7 +13738,7 @@
         <v>578</v>
       </c>
       <c r="D102" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E102">
         <v>0</v>
@@ -13758,7 +13755,7 @@
         <v>579</v>
       </c>
       <c r="D103" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E103">
         <v>0</v>
@@ -13775,7 +13772,7 @@
         <v>580</v>
       </c>
       <c r="D104" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E104">
         <v>0</v>
@@ -13792,7 +13789,7 @@
         <v>581</v>
       </c>
       <c r="D105" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E105">
         <v>0</v>
@@ -13809,7 +13806,7 @@
         <v>578</v>
       </c>
       <c r="D106" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E106">
         <v>0</v>
@@ -13826,7 +13823,7 @@
         <v>579</v>
       </c>
       <c r="D107" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E107">
         <v>0</v>
@@ -13843,7 +13840,7 @@
         <v>580</v>
       </c>
       <c r="D108" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E108">
         <v>0</v>
@@ -13860,7 +13857,7 @@
         <v>581</v>
       </c>
       <c r="D109" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E109">
         <v>0</v>
@@ -13877,7 +13874,7 @@
         <v>578</v>
       </c>
       <c r="D110" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E110">
         <v>0</v>
@@ -13894,7 +13891,7 @@
         <v>579</v>
       </c>
       <c r="D111" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E111">
         <v>0</v>
@@ -13911,7 +13908,7 @@
         <v>580</v>
       </c>
       <c r="D112" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E112">
         <v>0</v>
@@ -13928,7 +13925,7 @@
         <v>581</v>
       </c>
       <c r="D113" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E113">
         <v>0</v>
@@ -13945,7 +13942,7 @@
         <v>578</v>
       </c>
       <c r="D114" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E114">
         <v>0</v>
@@ -13962,7 +13959,7 @@
         <v>579</v>
       </c>
       <c r="D115" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E115">
         <v>0</v>
@@ -13979,7 +13976,7 @@
         <v>580</v>
       </c>
       <c r="D116" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E116">
         <v>0</v>
@@ -13996,7 +13993,7 @@
         <v>581</v>
       </c>
       <c r="D117" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E117">
         <v>0</v>
@@ -14010,7 +14007,7 @@
         <v>1</v>
       </c>
       <c r="C118" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D118" t="s">
         <v>582</v>
@@ -14027,7 +14024,7 @@
         <v>1</v>
       </c>
       <c r="C119" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D119" t="s">
         <v>583</v>
@@ -14044,7 +14041,7 @@
         <v>1</v>
       </c>
       <c r="C120" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D120" t="s">
         <v>584</v>
@@ -14061,7 +14058,7 @@
         <v>1</v>
       </c>
       <c r="C121" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D121" t="s">
         <v>585</v>
@@ -14078,7 +14075,7 @@
         <v>2</v>
       </c>
       <c r="C122" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D122" t="s">
         <v>582</v>
@@ -14095,7 +14092,7 @@
         <v>2</v>
       </c>
       <c r="C123" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D123" t="s">
         <v>583</v>
@@ -14112,7 +14109,7 @@
         <v>2</v>
       </c>
       <c r="C124" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D124" t="s">
         <v>584</v>
@@ -14129,7 +14126,7 @@
         <v>2</v>
       </c>
       <c r="C125" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D125" t="s">
         <v>585</v>
@@ -14146,7 +14143,7 @@
         <v>3</v>
       </c>
       <c r="C126" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D126" t="s">
         <v>582</v>
@@ -14163,7 +14160,7 @@
         <v>3</v>
       </c>
       <c r="C127" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D127" t="s">
         <v>583</v>
@@ -14180,7 +14177,7 @@
         <v>3</v>
       </c>
       <c r="C128" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D128" t="s">
         <v>584</v>
@@ -14197,7 +14194,7 @@
         <v>3</v>
       </c>
       <c r="C129" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D129" t="s">
         <v>585</v>
@@ -14214,7 +14211,7 @@
         <v>4</v>
       </c>
       <c r="C130" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D130" t="s">
         <v>582</v>
@@ -14231,7 +14228,7 @@
         <v>4</v>
       </c>
       <c r="C131" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D131" t="s">
         <v>583</v>
@@ -14248,7 +14245,7 @@
         <v>4</v>
       </c>
       <c r="C132" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D132" t="s">
         <v>584</v>
@@ -14265,7 +14262,7 @@
         <v>4</v>
       </c>
       <c r="C133" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D133" t="s">
         <v>585</v>
@@ -14282,7 +14279,7 @@
         <v>5</v>
       </c>
       <c r="C134" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D134" t="s">
         <v>582</v>
@@ -14299,7 +14296,7 @@
         <v>5</v>
       </c>
       <c r="C135" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D135" t="s">
         <v>583</v>
@@ -14316,7 +14313,7 @@
         <v>5</v>
       </c>
       <c r="C136" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D136" t="s">
         <v>584</v>
@@ -14333,7 +14330,7 @@
         <v>5</v>
       </c>
       <c r="C137" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D137" t="s">
         <v>585</v>
@@ -14350,7 +14347,7 @@
         <v>6</v>
       </c>
       <c r="C138" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D138" t="s">
         <v>582</v>
@@ -14367,7 +14364,7 @@
         <v>6</v>
       </c>
       <c r="C139" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D139" t="s">
         <v>583</v>
@@ -14384,7 +14381,7 @@
         <v>6</v>
       </c>
       <c r="C140" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D140" t="s">
         <v>584</v>
@@ -14401,7 +14398,7 @@
         <v>6</v>
       </c>
       <c r="C141" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D141" t="s">
         <v>585</v>
@@ -14418,7 +14415,7 @@
         <v>7</v>
       </c>
       <c r="C142" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D142" t="s">
         <v>582</v>
@@ -14435,7 +14432,7 @@
         <v>7</v>
       </c>
       <c r="C143" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D143" t="s">
         <v>583</v>
@@ -14452,7 +14449,7 @@
         <v>7</v>
       </c>
       <c r="C144" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D144" t="s">
         <v>584</v>
@@ -14469,7 +14466,7 @@
         <v>7</v>
       </c>
       <c r="C145" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D145" t="s">
         <v>585</v>
@@ -14486,7 +14483,7 @@
         <v>8</v>
       </c>
       <c r="C146" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D146" t="s">
         <v>582</v>
@@ -14503,7 +14500,7 @@
         <v>8</v>
       </c>
       <c r="C147" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D147" t="s">
         <v>583</v>
@@ -14520,7 +14517,7 @@
         <v>8</v>
       </c>
       <c r="C148" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D148" t="s">
         <v>584</v>
@@ -14537,7 +14534,7 @@
         <v>8</v>
       </c>
       <c r="C149" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D149" t="s">
         <v>585</v>
@@ -14554,7 +14551,7 @@
         <v>9</v>
       </c>
       <c r="C150" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D150" t="s">
         <v>582</v>
@@ -14571,7 +14568,7 @@
         <v>9</v>
       </c>
       <c r="C151" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D151" t="s">
         <v>583</v>
@@ -14588,7 +14585,7 @@
         <v>9</v>
       </c>
       <c r="C152" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D152" t="s">
         <v>584</v>
@@ -14605,7 +14602,7 @@
         <v>9</v>
       </c>
       <c r="C153" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D153" t="s">
         <v>585</v>
@@ -14622,7 +14619,7 @@
         <v>10</v>
       </c>
       <c r="C154" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D154" t="s">
         <v>582</v>
@@ -14639,7 +14636,7 @@
         <v>10</v>
       </c>
       <c r="C155" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D155" t="s">
         <v>583</v>
@@ -14656,7 +14653,7 @@
         <v>10</v>
       </c>
       <c r="C156" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D156" t="s">
         <v>584</v>
@@ -14673,7 +14670,7 @@
         <v>10</v>
       </c>
       <c r="C157" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D157" t="s">
         <v>585</v>
@@ -14690,7 +14687,7 @@
         <v>11</v>
       </c>
       <c r="C158" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D158" t="s">
         <v>582</v>
@@ -14707,7 +14704,7 @@
         <v>11</v>
       </c>
       <c r="C159" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D159" t="s">
         <v>583</v>
@@ -14724,7 +14721,7 @@
         <v>11</v>
       </c>
       <c r="C160" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D160" t="s">
         <v>584</v>
@@ -14741,7 +14738,7 @@
         <v>11</v>
       </c>
       <c r="C161" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D161" t="s">
         <v>585</v>
@@ -14758,7 +14755,7 @@
         <v>12</v>
       </c>
       <c r="C162" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D162" t="s">
         <v>582</v>
@@ -14775,7 +14772,7 @@
         <v>12</v>
       </c>
       <c r="C163" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D163" t="s">
         <v>583</v>
@@ -14792,7 +14789,7 @@
         <v>12</v>
       </c>
       <c r="C164" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D164" t="s">
         <v>584</v>
@@ -14809,7 +14806,7 @@
         <v>12</v>
       </c>
       <c r="C165" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D165" t="s">
         <v>585</v>
@@ -14826,7 +14823,7 @@
         <v>13</v>
       </c>
       <c r="C166" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D166" t="s">
         <v>582</v>
@@ -14843,7 +14840,7 @@
         <v>13</v>
       </c>
       <c r="C167" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D167" t="s">
         <v>583</v>
@@ -14860,7 +14857,7 @@
         <v>13</v>
       </c>
       <c r="C168" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D168" t="s">
         <v>584</v>
@@ -14877,7 +14874,7 @@
         <v>13</v>
       </c>
       <c r="C169" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D169" t="s">
         <v>585</v>
@@ -14894,7 +14891,7 @@
         <v>14</v>
       </c>
       <c r="C170" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D170" t="s">
         <v>582</v>
@@ -14911,7 +14908,7 @@
         <v>14</v>
       </c>
       <c r="C171" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D171" t="s">
         <v>583</v>
@@ -14928,7 +14925,7 @@
         <v>14</v>
       </c>
       <c r="C172" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D172" t="s">
         <v>584</v>
@@ -14945,7 +14942,7 @@
         <v>14</v>
       </c>
       <c r="C173" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D173" t="s">
         <v>585</v>
@@ -14962,7 +14959,7 @@
         <v>15</v>
       </c>
       <c r="C174" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D174" t="s">
         <v>582</v>
@@ -14979,7 +14976,7 @@
         <v>15</v>
       </c>
       <c r="C175" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D175" t="s">
         <v>583</v>
@@ -14996,7 +14993,7 @@
         <v>15</v>
       </c>
       <c r="C176" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D176" t="s">
         <v>584</v>
@@ -15013,7 +15010,7 @@
         <v>15</v>
       </c>
       <c r="C177" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D177" t="s">
         <v>585</v>
@@ -15030,7 +15027,7 @@
         <v>16</v>
       </c>
       <c r="C178" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D178" t="s">
         <v>582</v>
@@ -15047,7 +15044,7 @@
         <v>16</v>
       </c>
       <c r="C179" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D179" t="s">
         <v>583</v>
@@ -15064,7 +15061,7 @@
         <v>16</v>
       </c>
       <c r="C180" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D180" t="s">
         <v>584</v>
@@ -15081,7 +15078,7 @@
         <v>16</v>
       </c>
       <c r="C181" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D181" t="s">
         <v>585</v>
@@ -15098,7 +15095,7 @@
         <v>17</v>
       </c>
       <c r="C182" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D182" t="s">
         <v>582</v>
@@ -15115,7 +15112,7 @@
         <v>17</v>
       </c>
       <c r="C183" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D183" t="s">
         <v>583</v>
@@ -15132,7 +15129,7 @@
         <v>17</v>
       </c>
       <c r="C184" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D184" t="s">
         <v>584</v>
@@ -15149,7 +15146,7 @@
         <v>17</v>
       </c>
       <c r="C185" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D185" t="s">
         <v>585</v>
@@ -15166,7 +15163,7 @@
         <v>18</v>
       </c>
       <c r="C186" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D186" t="s">
         <v>582</v>
@@ -15183,7 +15180,7 @@
         <v>18</v>
       </c>
       <c r="C187" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D187" t="s">
         <v>583</v>
@@ -15200,7 +15197,7 @@
         <v>18</v>
       </c>
       <c r="C188" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D188" t="s">
         <v>584</v>
@@ -15217,7 +15214,7 @@
         <v>18</v>
       </c>
       <c r="C189" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D189" t="s">
         <v>585</v>
@@ -15234,7 +15231,7 @@
         <v>19</v>
       </c>
       <c r="C190" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D190" t="s">
         <v>582</v>
@@ -15251,7 +15248,7 @@
         <v>19</v>
       </c>
       <c r="C191" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D191" t="s">
         <v>583</v>
@@ -15268,7 +15265,7 @@
         <v>19</v>
       </c>
       <c r="C192" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D192" t="s">
         <v>584</v>
@@ -15285,7 +15282,7 @@
         <v>19</v>
       </c>
       <c r="C193" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D193" t="s">
         <v>585</v>
@@ -15302,7 +15299,7 @@
         <v>20</v>
       </c>
       <c r="C194" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D194" t="s">
         <v>582</v>
@@ -15319,7 +15316,7 @@
         <v>20</v>
       </c>
       <c r="C195" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D195" t="s">
         <v>583</v>
@@ -15336,7 +15333,7 @@
         <v>20</v>
       </c>
       <c r="C196" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D196" t="s">
         <v>584</v>
@@ -15353,7 +15350,7 @@
         <v>20</v>
       </c>
       <c r="C197" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D197" t="s">
         <v>585</v>
@@ -15370,7 +15367,7 @@
         <v>21</v>
       </c>
       <c r="C198" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D198" t="s">
         <v>582</v>
@@ -15387,7 +15384,7 @@
         <v>21</v>
       </c>
       <c r="C199" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D199" t="s">
         <v>583</v>
@@ -15404,7 +15401,7 @@
         <v>21</v>
       </c>
       <c r="C200" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D200" t="s">
         <v>584</v>
@@ -15421,7 +15418,7 @@
         <v>21</v>
       </c>
       <c r="C201" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D201" t="s">
         <v>585</v>
@@ -15438,7 +15435,7 @@
         <v>22</v>
       </c>
       <c r="C202" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D202" t="s">
         <v>582</v>
@@ -15455,7 +15452,7 @@
         <v>22</v>
       </c>
       <c r="C203" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D203" t="s">
         <v>583</v>
@@ -15472,7 +15469,7 @@
         <v>22</v>
       </c>
       <c r="C204" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D204" t="s">
         <v>584</v>
@@ -15489,7 +15486,7 @@
         <v>22</v>
       </c>
       <c r="C205" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D205" t="s">
         <v>585</v>
@@ -15506,7 +15503,7 @@
         <v>23</v>
       </c>
       <c r="C206" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D206" t="s">
         <v>582</v>
@@ -15523,7 +15520,7 @@
         <v>23</v>
       </c>
       <c r="C207" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D207" t="s">
         <v>583</v>
@@ -15540,7 +15537,7 @@
         <v>23</v>
       </c>
       <c r="C208" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D208" t="s">
         <v>584</v>
@@ -15557,7 +15554,7 @@
         <v>23</v>
       </c>
       <c r="C209" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D209" t="s">
         <v>585</v>

</xml_diff>